<commit_message>
A few small mistakes that I found.
</commit_message>
<xml_diff>
--- a/examples/leas_survey_example.xlsx
+++ b/examples/leas_survey_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2dde9360acc1c89/Dokumente/GitHub/veta/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_CDBBE437E243E8529B4F26CD8B44E6735DA2ABCA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0845E88-1A5B-45AC-892B-BDDBA1D1AE28}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_CDBBE437E243E8529B4F26CD8B44E6735DA2ABCA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B962C785-CB68-4246-96BC-DA22764EAA3B}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t xml:space="preserve">Person </t>
   </si>
@@ -60,42 +60,24 @@
     <t>Sein ganzer Körper würde zittern.</t>
   </si>
   <si>
-    <t>Ich würde mich nicht gut fühlen</t>
-  </si>
-  <si>
     <t>Er würde sich schlecht fühlen.</t>
   </si>
   <si>
-    <t>Sie ist glücklich</t>
-  </si>
-  <si>
     <t>Ich will nach Hause, denn ich habe Angst.</t>
   </si>
   <si>
     <t>Sie hat auch Angst und will nach Hause.</t>
   </si>
   <si>
-    <t>Ich bin traurig und wütend</t>
-  </si>
-  <si>
     <t>Ich würde weinen, weil ich so glücklich bin.</t>
   </si>
   <si>
-    <t>Meine Freundin würde sich gut fühlen</t>
-  </si>
-  <si>
     <t>An so etwas glaube ich nicht.</t>
   </si>
   <si>
     <t>Ich weiß nicht, wie sie sich fühlen würde.</t>
   </si>
   <si>
-    <t>Ich würde Schmerz verspüren</t>
-  </si>
-  <si>
-    <t>Er fühlt sich schuldig</t>
-  </si>
-  <si>
     <t>Ich wäre erleichtert.</t>
   </si>
   <si>
@@ -123,12 +105,6 @@
     <t xml:space="preserve">Er scheint nichts zu merken. </t>
   </si>
   <si>
-    <t xml:space="preserve">Gut </t>
-  </si>
-  <si>
-    <t>Glücklich</t>
-  </si>
-  <si>
     <t>Ich würde Schmerz verspüren.</t>
   </si>
   <si>
@@ -141,9 +117,6 @@
     <t xml:space="preserve">Er kann mich nicht verstehen. </t>
   </si>
   <si>
-    <t>Ich bin glücklich und erleichtert</t>
-  </si>
-  <si>
     <t>Er ist wütend und enttäuscht.</t>
   </si>
   <si>
@@ -153,13 +126,37 @@
     <t>Sie bleibt gelassen.</t>
   </si>
   <si>
-    <t>Schlecht</t>
-  </si>
-  <si>
-    <t>Nichts</t>
-  </si>
-  <si>
-    <t>Ich will, dass sie mich umarmt</t>
+    <t>Ich würde mich nicht gut fühlen.</t>
+  </si>
+  <si>
+    <t>Ich will, dass sie mich umarmt.</t>
+  </si>
+  <si>
+    <t>Sie ist glücklich.</t>
+  </si>
+  <si>
+    <t>Ich bin traurig und wütend.</t>
+  </si>
+  <si>
+    <t>Meine Freundin würde sich gut fühlen.</t>
+  </si>
+  <si>
+    <t>Er fühlt sich schuldig.</t>
+  </si>
+  <si>
+    <t>Gut .</t>
+  </si>
+  <si>
+    <t>Glücklich.</t>
+  </si>
+  <si>
+    <t>Ich bin glücklich und erleichtert.</t>
+  </si>
+  <si>
+    <t>Schlecht.</t>
+  </si>
+  <si>
+    <t>Nichts.</t>
   </si>
 </sst>
 </file>
@@ -212,6 +209,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,10 +575,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
@@ -585,10 +586,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
@@ -596,10 +597,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
@@ -607,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.35">
@@ -615,10 +616,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
@@ -626,10 +627,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
@@ -637,10 +638,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
@@ -648,10 +649,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
@@ -670,10 +671,10 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.35">
@@ -681,7 +682,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
@@ -689,10 +690,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
@@ -700,10 +701,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -711,10 +712,10 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -722,10 +723,10 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -733,10 +734,10 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -744,10 +745,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -755,10 +756,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>